<commit_message>
Update to the thesis paper and data sheet.
</commit_message>
<xml_diff>
--- a/data_survey.xlsx
+++ b/data_survey.xlsx
@@ -63,17 +63,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,17 +87,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -121,20 +109,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,13 +1035,13 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1485,23 +1470,23 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="2">
-        <v>4</v>
-      </c>
-      <c r="C51" s="2">
-        <v>5</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2">
-        <v>3</v>
-      </c>
-      <c r="F51" s="2">
-        <v>4</v>
-      </c>
-      <c r="G51" s="2">
-        <v>3</v>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,7 +1575,7 @@
       </c>
       <c r="B56">
         <f>SUM($B31:$B55)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C56">
         <f>SUM($C31:$C55)</f>
@@ -1598,19 +1583,19 @@
       </c>
       <c r="D56">
         <f>SUM($D31:$D55)</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E56">
         <f>SUM($E31:$E55)</f>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F56">
         <f>SUM($F31:$F55)</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G56">
         <f>SUM($G31:$G55)</f>
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1619,7 +1604,7 @@
       </c>
       <c r="B57">
         <f>AVERAGE($B31:$B55, $B31:$B55)</f>
-        <v>3.96</v>
+        <v>4</v>
       </c>
       <c r="C57">
         <f>AVERAGE($C31:$C55, $C31:$C55)</f>
@@ -1627,19 +1612,19 @@
       </c>
       <c r="D57">
         <f>AVERAGE($D31:$D55, $D31:$D55)</f>
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="E57">
         <f>AVERAGE($E31:$E55, $E31:$E55)</f>
-        <v>3.6</v>
+        <v>3.68</v>
       </c>
       <c r="F57">
         <f>AVERAGE($F31:$F55, $F31:$F55)</f>
-        <v>3.84</v>
+        <v>3.88</v>
       </c>
       <c r="G57">
         <f>AVERAGE($G31:$G55, $G31:$G55)</f>
-        <v>3.84</v>
+        <v>3.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>